<commit_message>
ReportErrors, Fixed Report Steel
</commit_message>
<xml_diff>
--- a/SZMK.Desktop/bin/Debug/Program/Templates/ReportSteelTemplate.xlsx
+++ b/SZMK.Desktop/bin/Debug/Program/Templates/ReportSteelTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE74702D-CCFE-4958-8932-439E32A3F227}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320DCAD2-2C3B-49F5-B616-A1A10333E563}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Марка стали</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Отчет выборки металла</t>
+  </si>
+  <si>
+    <t>ГОСТ</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,6 +407,9 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>